<commit_message>
update API khảo sát
</commit_message>
<xml_diff>
--- a/DOC/API.xlsx
+++ b/DOC/API.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
   <si>
     <t>STT</t>
   </si>
@@ -315,6 +315,54 @@
   </si>
   <si>
     <t>http://13.250.191.59:9000</t>
+  </si>
+  <si>
+    <t>Insert khảo sát</t>
+  </si>
+  <si>
+    <t>Sửa khảo sát</t>
+  </si>
+  <si>
+    <t>Tìm kiếm khảo sát</t>
+  </si>
+  <si>
+    <t>/api/v1/surveys</t>
+  </si>
+  <si>
+    <t>/api/v1/surveys/search</t>
+  </si>
+  <si>
+    <t>Insert câu hỏi khảo sát</t>
+  </si>
+  <si>
+    <t>/api/v1/survey/answers/search</t>
+  </si>
+  <si>
+    <t>/api/v1/survey/answers</t>
+  </si>
+  <si>
+    <t>/api/v1/survey/questions/search</t>
+  </si>
+  <si>
+    <t>/api/v1/survey/questions</t>
+  </si>
+  <si>
+    <t>Sửa câu hỏi khảo sát</t>
+  </si>
+  <si>
+    <t>Tìm kiếm câu hỏi khảo sát</t>
+  </si>
+  <si>
+    <t>Insert câu trả lời khảo sát</t>
+  </si>
+  <si>
+    <t>Sửa câu trả lời khảo sát</t>
+  </si>
+  <si>
+    <t>Tìm kiếm câu trả lời khảo sát</t>
+  </si>
+  <si>
+    <t>Tương tự như các API trước</t>
   </si>
 </sst>
 </file>
@@ -411,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -427,7 +475,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -730,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1229,7 @@
       <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1195,9 +1248,172 @@
         <v>52</v>
       </c>
     </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:C20"/>
+    <mergeCell ref="C22:C31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>